<commit_message>
add files 23 sept
</commit_message>
<xml_diff>
--- a/Evaluation_Results/Final_TestFiles_12thSeptember_FewShotTest_Broad_Count/detailed_category_results_DeepSeekV3_4_shot.xlsx
+++ b/Evaluation_Results/Final_TestFiles_12thSeptember_FewShotTest_Broad_Count/detailed_category_results_DeepSeekV3_4_shot.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1021,6 +1021,502 @@
         <v>57</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>09/13/2025</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>DeepSeekV3</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Soil</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>12</v>
+      </c>
+      <c r="F10" t="n">
+        <v>61</v>
+      </c>
+      <c r="G10" t="n">
+        <v>35</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.1643835616438356</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.2553191489361702</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K10" t="n">
+        <v>47</v>
+      </c>
+      <c r="L10" t="n">
+        <v>18</v>
+      </c>
+      <c r="M10" t="n">
+        <v>55</v>
+      </c>
+      <c r="N10" t="n">
+        <v>29</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.2465753424657534</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.3829787234042553</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="R10" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>09/13/2025</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>DeepSeekV3</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>city</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>9</v>
+      </c>
+      <c r="F11" t="n">
+        <v>9</v>
+      </c>
+      <c r="G11" t="n">
+        <v>8</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.5294117647058824</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.5142857142857143</v>
+      </c>
+      <c r="K11" t="n">
+        <v>17</v>
+      </c>
+      <c r="L11" t="n">
+        <v>9</v>
+      </c>
+      <c r="M11" t="n">
+        <v>9</v>
+      </c>
+      <c r="N11" t="n">
+        <v>8</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.5294117647058824</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.5142857142857143</v>
+      </c>
+      <c r="R11" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>09/13/2025</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DeepSeekV3</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>4</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>country</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>9</v>
+      </c>
+      <c r="F12" t="n">
+        <v>7</v>
+      </c>
+      <c r="G12" t="n">
+        <v>13</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.5625</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.4090909090909091</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.4736842105263158</v>
+      </c>
+      <c r="K12" t="n">
+        <v>22</v>
+      </c>
+      <c r="L12" t="n">
+        <v>9</v>
+      </c>
+      <c r="M12" t="n">
+        <v>7</v>
+      </c>
+      <c r="N12" t="n">
+        <v>13</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.5625</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.4090909090909091</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.4736842105263158</v>
+      </c>
+      <c r="R12" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>09/13/2025</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>DeepSeekV3</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>4</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>cropSpecies</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>30</v>
+      </c>
+      <c r="F13" t="n">
+        <v>20</v>
+      </c>
+      <c r="G13" t="n">
+        <v>51</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.3703703703703703</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.4580152671755725</v>
+      </c>
+      <c r="K13" t="n">
+        <v>81</v>
+      </c>
+      <c r="L13" t="n">
+        <v>37</v>
+      </c>
+      <c r="M13" t="n">
+        <v>13</v>
+      </c>
+      <c r="N13" t="n">
+        <v>44</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.4567901234567901</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.564885496183206</v>
+      </c>
+      <c r="R13" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>09/13/2025</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>DeepSeekV3</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>4</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>duration</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>3</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" t="n">
+        <v>19</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.1363636363636364</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.2307692307692308</v>
+      </c>
+      <c r="K14" t="n">
+        <v>22</v>
+      </c>
+      <c r="L14" t="n">
+        <v>4</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>18</v>
+      </c>
+      <c r="O14" t="n">
+        <v>1</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.1818181818181818</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.3076923076923077</v>
+      </c>
+      <c r="R14" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>09/13/2025</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>DeepSeekV3</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>4</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>endTime</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>20</v>
+      </c>
+      <c r="F15" t="n">
+        <v>14</v>
+      </c>
+      <c r="G15" t="n">
+        <v>11</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.5882352941176471</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.6451612903225806</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.6153846153846154</v>
+      </c>
+      <c r="K15" t="n">
+        <v>31</v>
+      </c>
+      <c r="L15" t="n">
+        <v>21</v>
+      </c>
+      <c r="M15" t="n">
+        <v>13</v>
+      </c>
+      <c r="N15" t="n">
+        <v>10</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.6176470588235294</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.6774193548387096</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.6461538461538462</v>
+      </c>
+      <c r="R15" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>09/13/2025</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>DeepSeekV3</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>4</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>region</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>3</v>
+      </c>
+      <c r="F16" t="n">
+        <v>3</v>
+      </c>
+      <c r="G16" t="n">
+        <v>9</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="K16" t="n">
+        <v>12</v>
+      </c>
+      <c r="L16" t="n">
+        <v>3</v>
+      </c>
+      <c r="M16" t="n">
+        <v>3</v>
+      </c>
+      <c r="N16" t="n">
+        <v>9</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="R16" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>09/13/2025</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>DeepSeekV3</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>4</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>startTime</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>31</v>
+      </c>
+      <c r="F17" t="n">
+        <v>4</v>
+      </c>
+      <c r="G17" t="n">
+        <v>26</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.8857142857142857</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.543859649122807</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.673913043478261</v>
+      </c>
+      <c r="K17" t="n">
+        <v>57</v>
+      </c>
+      <c r="L17" t="n">
+        <v>32</v>
+      </c>
+      <c r="M17" t="n">
+        <v>3</v>
+      </c>
+      <c r="N17" t="n">
+        <v>25</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.9142857142857143</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.5614035087719298</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.6956521739130436</v>
+      </c>
+      <c r="R17" t="n">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>